<commit_message>
Outils d'import Validation des données importées
Il y avais certains problèmes sur la validation des données
</commit_message>
<xml_diff>
--- a/Fixtures.xlsx
+++ b/Fixtures.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
-  <workbookPr codeName="ThisWorkbook"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\xampp\htdocs\new_age\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\xampp\htdocs\new_age\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25755" windowHeight="9465" firstSheet="1" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" tabRatio="993" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Liste des Composantes" sheetId="1" r:id="rId1"/>
@@ -19,12 +19,17 @@
     <sheet name="Liste Unitées d'enseignement" sheetId="5" r:id="rId5"/>
     <sheet name="Liste des Cours" sheetId="6" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="0" iterateDelta="1E-4"/>
+  <extLst>
+    <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
+      <loext:extCalcPr stringRefSyntax="ExcelA1"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="304" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="390" uniqueCount="115">
   <si>
     <t>Composantes</t>
   </si>
@@ -215,10 +220,10 @@
     <t>Description</t>
   </si>
   <si>
-    <t>M1-INFO</t>
-  </si>
-  <si>
-    <t>M2-INFO</t>
+    <t>M1-INFO-GL</t>
+  </si>
+  <si>
+    <t>M2-INFO-GL</t>
   </si>
   <si>
     <t>Unitées d'enseignements</t>
@@ -230,25 +235,109 @@
     <t>ACO</t>
   </si>
   <si>
+    <t>Analyse et Conception Objet</t>
+  </si>
+  <si>
+    <t>COMP</t>
+  </si>
+  <si>
+    <t>Compilation</t>
+  </si>
+  <si>
+    <t>SE</t>
+  </si>
+  <si>
+    <t>Systèmes d’exploitation</t>
+  </si>
+  <si>
+    <t>GPL</t>
+  </si>
+  <si>
+    <t>Gestion de projet logiciels</t>
+  </si>
+  <si>
+    <t>SECU</t>
+  </si>
+  <si>
+    <t>Introduction à la sécurité informatique</t>
+  </si>
+  <si>
+    <t>BD</t>
+  </si>
+  <si>
+    <t>Base de données : aspects techniques</t>
+  </si>
+  <si>
+    <t>AA</t>
+  </si>
+  <si>
+    <t>Algorithmique avancée</t>
+  </si>
+  <si>
+    <t>SEM</t>
+  </si>
+  <si>
+    <t>Semantique</t>
+  </si>
+  <si>
     <t>ACF</t>
   </si>
   <si>
-    <t>COMP</t>
+    <t>Analyse et conception formelle</t>
+  </si>
+  <si>
+    <t>MRI</t>
+  </si>
+  <si>
+    <t>Mécanismes des réseaux informatiques</t>
   </si>
   <si>
     <t>MFDS</t>
   </si>
   <si>
+    <t>Méthodes formelles pour le développement de logiciels sûrs</t>
+  </si>
+  <si>
+    <t>IA</t>
+  </si>
+  <si>
+    <t>Intelligence artificielle</t>
+  </si>
+  <si>
+    <t>IDM</t>
+  </si>
+  <si>
+    <t>Ingénieurie dirigée des modèles</t>
+  </si>
+  <si>
+    <t>VV</t>
+  </si>
+  <si>
+    <t>Validation et vérification</t>
+  </si>
+  <si>
+    <t>DOC</t>
+  </si>
+  <si>
+    <t>Documents structurés : concepts et langages</t>
+  </si>
+  <si>
+    <t>TAA</t>
+  </si>
+  <si>
+    <t>Techniques avancées pour la construction d’architectures logicielles</t>
+  </si>
+  <si>
+    <t>GLI</t>
+  </si>
+  <si>
+    <t>Génie logiciel pour les IHM</t>
+  </si>
+  <si>
     <t>AOC</t>
   </si>
   <si>
-    <t>RSIP</t>
-  </si>
-  <si>
-    <t>ANGLAIS</t>
-  </si>
-  <si>
-    <t>ECO</t>
+    <t>Architecture à objets canoniques</t>
   </si>
   <si>
     <t>Cours</t>
@@ -272,31 +361,19 @@
     <t>CM</t>
   </si>
   <si>
+    <t>Cours magistral dispensé en anglais</t>
+  </si>
+  <si>
     <t>TD</t>
   </si>
   <si>
+    <t>3 groupes GL et 3 groupes MIAGE</t>
+  </si>
+  <si>
     <t>TP</t>
   </si>
   <si>
-    <t>Compilation</t>
-  </si>
-  <si>
-    <t>Méthode formelle de déduction…</t>
-  </si>
-  <si>
-    <t>Communication</t>
-  </si>
-  <si>
-    <t>Anglais</t>
-  </si>
-  <si>
-    <t>Economie</t>
-  </si>
-  <si>
-    <t>ACO Conception Objet</t>
-  </si>
-  <si>
-    <t>Preuve formelle</t>
+    <t>0631041660</t>
   </si>
 </sst>
 </file>
@@ -308,6 +385,8 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -328,16 +407,16 @@
     </border>
     <border>
       <left style="medium">
-        <color rgb="FF000000"/>
+        <color auto="1"/>
       </left>
       <right style="medium">
-        <color rgb="FF000000"/>
+        <color auto="1"/>
       </right>
       <top style="medium">
-        <color rgb="FF000000"/>
+        <color auto="1"/>
       </top>
       <bottom style="medium">
-        <color rgb="FF000000"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -345,16 +424,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -367,7 +448,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -377,39 +458,39 @@
         <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="1F497D"/>
+        <a:srgbClr val="44546A"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="EEECE1"/>
+        <a:srgbClr val="E7E6E6"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="4F81BD"/>
+        <a:srgbClr val="5B9BD5"/>
       </a:accent1>
       <a:accent2>
-        <a:srgbClr val="C0504D"/>
+        <a:srgbClr val="ED7D31"/>
       </a:accent2>
       <a:accent3>
-        <a:srgbClr val="9BBB59"/>
+        <a:srgbClr val="A5A5A5"/>
       </a:accent3>
       <a:accent4>
-        <a:srgbClr val="8064A2"/>
+        <a:srgbClr val="FFC000"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="4BACC6"/>
+        <a:srgbClr val="4472C4"/>
       </a:accent5>
       <a:accent6>
-        <a:srgbClr val="F79646"/>
+        <a:srgbClr val="70AD47"/>
       </a:accent6>
       <a:hlink>
-        <a:srgbClr val="0000FF"/>
+        <a:srgbClr val="0563C1"/>
       </a:hlink>
       <a:folHlink>
-        <a:srgbClr val="800080"/>
+        <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -444,7 +525,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -488,166 +569,142 @@
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:tint val="50000"/>
-                <a:satMod val="300000"/>
+                <a:lumMod val="110000"/>
+                <a:satMod val="105000"/>
+                <a:tint val="67000"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="35000">
+            <a:gs pos="50000">
               <a:schemeClr val="phClr">
-                <a:tint val="37000"/>
-                <a:satMod val="300000"/>
+                <a:lumMod val="105000"/>
+                <a:satMod val="103000"/>
+                <a:tint val="73000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:tint val="15000"/>
-                <a:satMod val="350000"/>
+                <a:lumMod val="105000"/>
+                <a:satMod val="109000"/>
+                <a:tint val="81000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="16200000" scaled="1"/>
+          <a:lin ang="5400000" scaled="0"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:shade val="51000"/>
-                <a:satMod val="130000"/>
+                <a:satMod val="103000"/>
+                <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="80000">
+            <a:gs pos="50000">
               <a:schemeClr val="phClr">
-                <a:shade val="93000"/>
-                <a:satMod val="130000"/>
+                <a:satMod val="110000"/>
+                <a:lumMod val="100000"/>
+                <a:shade val="100000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:shade val="94000"/>
-                <a:satMod val="135000"/>
+                <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
+                <a:shade val="78000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="16200000" scaled="0"/>
+          <a:lin ang="5400000" scaled="0"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr">
-              <a:shade val="95000"/>
-              <a:satMod val="105000"/>
-            </a:schemeClr>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-        </a:ln>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
         </a:ln>
       </a:lnStyleLst>
       <a:effectStyleLst>
         <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
               <a:srgbClr val="000000">
-                <a:alpha val="38000"/>
+                <a:alpha val="63000"/>
               </a:srgbClr>
             </a:outerShdw>
           </a:effectLst>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
-              <a:srgbClr val="000000">
-                <a:alpha val="35000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
-              <a:srgbClr val="000000">
-                <a:alpha val="35000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
-          <a:scene3d>
-            <a:camera prst="orthographicFront">
-              <a:rot lat="0" lon="0" rev="0"/>
-            </a:camera>
-            <a:lightRig rig="threePt" dir="t">
-              <a:rot lat="0" lon="0" rev="1200000"/>
-            </a:lightRig>
-          </a:scene3d>
-          <a:sp3d>
-            <a:bevelT w="63500" h="25400"/>
-          </a:sp3d>
         </a:effectStyle>
       </a:effectStyleLst>
       <a:bgFillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:tint val="95000"/>
+            <a:satMod val="170000"/>
+          </a:schemeClr>
+        </a:solidFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:tint val="40000"/>
-                <a:satMod val="350000"/>
+                <a:tint val="93000"/>
+                <a:satMod val="150000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="40000">
+            <a:gs pos="50000">
               <a:schemeClr val="phClr">
-                <a:tint val="45000"/>
-                <a:shade val="99000"/>
-                <a:satMod val="350000"/>
+                <a:tint val="98000"/>
+                <a:satMod val="130000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:shade val="20000"/>
-                <a:satMod val="255000"/>
+                <a:shade val="63000"/>
+                <a:satMod val="120000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:path path="circle">
-            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
-          </a:path>
-        </a:gradFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:tint val="80000"/>
-                <a:satMod val="300000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:shade val="30000"/>
-                <a:satMod val="200000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:path path="circle">
-            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
-          </a:path>
+          <a:lin ang="5400000" scaled="0"/>
         </a:gradFill>
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
   <a:extraClrSchemeLst/>
+  <a:extLst>
+    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+    </a:ext>
+  </a:extLst>
 </a:theme>
 </file>
 
@@ -655,21 +712,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="3.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="3.42578125"/>
+    <col min="2" max="2" width="7.140625"/>
+    <col min="3" max="1025" width="9.42578125"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2"/>
+      <c r="B1" s="3"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -696,11 +754,11 @@
       </c>
     </row>
   </sheetData>
-  <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <mergeCells count="1">
     <mergeCell ref="A1:B1"/>
   </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
 </file>
 
@@ -708,23 +766,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="3.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="38.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="33" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="3.42578125"/>
+    <col min="2" max="2" width="40.140625"/>
+    <col min="3" max="3" width="34.140625"/>
+    <col min="4" max="1025" width="9.42578125"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -815,11 +874,11 @@
       </c>
     </row>
   </sheetData>
-  <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <mergeCells count="1">
     <mergeCell ref="A1:C1"/>
   </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
 </file>
 
@@ -827,59 +886,60 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="Q3" sqref="Q3"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="3.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="21.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="84.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="3.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="27" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="3.42578125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="27" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="3.42578125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="29.42578125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="3.42578125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="3.42578125"/>
+    <col min="3" max="3" width="7.140625"/>
+    <col min="4" max="4" width="21.85546875"/>
+    <col min="5" max="5" width="12.140625"/>
+    <col min="6" max="6" width="21.85546875"/>
+    <col min="7" max="7" width="87.85546875"/>
+    <col min="8" max="8" width="8.42578125"/>
+    <col min="9" max="9" width="17"/>
+    <col min="10" max="10" width="3.42578125"/>
+    <col min="11" max="11" width="28"/>
+    <col min="12" max="12" width="3.42578125"/>
+    <col min="13" max="13" width="28"/>
+    <col min="14" max="14" width="3.42578125"/>
+    <col min="15" max="15" width="30.42578125"/>
+    <col min="16" max="16" width="3.42578125"/>
+    <col min="17" max="17" width="18.140625"/>
+    <col min="18" max="1025" width="9.42578125"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
-      <c r="I1" s="2"/>
-      <c r="J1" s="2"/>
-      <c r="K1" s="2"/>
-      <c r="L1" s="2"/>
-      <c r="M1" s="2"/>
-      <c r="N1" s="2"/>
-      <c r="O1" s="2"/>
-      <c r="P1" s="2"/>
-      <c r="Q1" s="2"/>
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="3"/>
+      <c r="I1" s="3"/>
+      <c r="J1" s="3"/>
+      <c r="K1" s="3"/>
+      <c r="L1" s="3"/>
+      <c r="M1" s="3"/>
+      <c r="N1" s="3"/>
+      <c r="O1" s="3"/>
+      <c r="P1" s="3"/>
+      <c r="Q1" s="3"/>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="C2" s="2"/>
+      <c r="C2" s="3"/>
       <c r="D2" s="1" t="s">
         <v>2</v>
       </c>
@@ -898,22 +958,22 @@
       <c r="I2" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="J2" s="2" t="s">
+      <c r="J2" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="K2" s="2"/>
-      <c r="L2" s="2" t="s">
+      <c r="K2" s="3"/>
+      <c r="L2" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="M2" s="2"/>
-      <c r="N2" s="2" t="s">
+      <c r="M2" s="3"/>
+      <c r="N2" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="O2" s="2"/>
-      <c r="P2" s="2" t="s">
+      <c r="O2" s="3"/>
+      <c r="P2" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="Q2" s="2"/>
+      <c r="Q2" s="3"/>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
@@ -1050,8 +1110,8 @@
       <c r="P5">
         <v>2</v>
       </c>
-      <c r="Q5">
-        <v>33222113344</v>
+      <c r="Q5" s="4" t="s">
+        <v>114</v>
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.25">
@@ -1150,8 +1210,8 @@
       <c r="P7">
         <v>2</v>
       </c>
-      <c r="Q7">
-        <v>33222113344</v>
+      <c r="Q7" s="4" t="s">
+        <v>114</v>
       </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
@@ -1791,7 +1851,6 @@
       </c>
     </row>
   </sheetData>
-  <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <mergeCells count="6">
     <mergeCell ref="A1:Q1"/>
     <mergeCell ref="B2:C2"/>
@@ -1800,7 +1859,8 @@
     <mergeCell ref="N2:O2"/>
     <mergeCell ref="P2:Q2"/>
   </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1808,27 +1868,28 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="P7" sqref="P7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="3.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="3.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="3.42578125"/>
+    <col min="2" max="2" width="7.140625"/>
+    <col min="3" max="3" width="3.42578125"/>
+    <col min="4" max="4" width="9.5703125"/>
+    <col min="5" max="5" width="14.42578125"/>
+    <col min="6" max="1025" width="9.42578125"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -1837,11 +1898,11 @@
       <c r="B2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
@@ -1866,7 +1927,7 @@
       <c r="C4">
         <v>1</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="2" t="s">
         <v>63</v>
       </c>
     </row>
@@ -1885,47 +1946,49 @@
       </c>
     </row>
   </sheetData>
-  <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <mergeCells count="2">
     <mergeCell ref="A1:E1"/>
     <mergeCell ref="C2:E2"/>
   </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:E21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="3.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="31.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="3.42578125"/>
+    <col min="3" max="3" width="12.85546875"/>
+    <col min="4" max="4" width="9.5703125"/>
+    <col min="5" max="5" width="55"/>
+    <col min="6" max="1025" width="9.42578125"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="C2" s="2"/>
+      <c r="C2" s="3"/>
       <c r="D2" s="1" t="s">
         <v>2</v>
       </c>
@@ -1945,199 +2008,374 @@
       <c r="E3" s="1"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>1</v>
-      </c>
-      <c r="B4">
-        <v>1</v>
-      </c>
-      <c r="C4" t="s">
+      <c r="A4" s="2">
+        <v>1</v>
+      </c>
+      <c r="B4" s="2">
+        <v>1</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" s="2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="2">
+        <v>2</v>
+      </c>
+      <c r="B5" s="2">
+        <v>1</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="2">
+        <v>3</v>
+      </c>
+      <c r="B6" s="2">
+        <v>1</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="2">
+        <v>4</v>
+      </c>
+      <c r="B7" s="2">
+        <v>1</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="2">
+        <v>5</v>
+      </c>
+      <c r="B8" s="2">
+        <v>1</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="E8" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="2">
+        <v>6</v>
+      </c>
+      <c r="B9" s="2">
+        <v>1</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="2">
+        <v>7</v>
+      </c>
+      <c r="B10" s="2">
+        <v>1</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="2">
+        <v>8</v>
+      </c>
+      <c r="B11" s="2">
+        <v>1</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="2">
+        <v>9</v>
+      </c>
+      <c r="B12" s="2">
+        <v>1</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="2">
+        <v>10</v>
+      </c>
+      <c r="B13" s="2">
+        <v>1</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="2">
+        <v>11</v>
+      </c>
+      <c r="B14" s="2">
+        <v>1</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="2">
+        <v>12</v>
+      </c>
+      <c r="B15" s="2">
+        <v>1</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="D15" s="2" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>2</v>
-      </c>
-      <c r="B5">
-        <v>1</v>
-      </c>
-      <c r="C5" t="s">
-        <v>63</v>
-      </c>
-      <c r="D5" t="s">
-        <v>68</v>
-      </c>
-      <c r="E5" t="s">
+      <c r="E15" s="2" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>3</v>
-      </c>
-      <c r="B6">
-        <v>1</v>
-      </c>
-      <c r="C6" t="s">
-        <v>63</v>
-      </c>
-      <c r="D6" t="s">
-        <v>69</v>
-      </c>
-      <c r="E6" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>4</v>
-      </c>
-      <c r="B7">
-        <v>1</v>
-      </c>
-      <c r="C7" t="s">
-        <v>63</v>
-      </c>
-      <c r="D7" t="s">
-        <v>70</v>
-      </c>
-      <c r="E7" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>5</v>
-      </c>
-      <c r="B8">
-        <v>2</v>
-      </c>
-      <c r="C8" t="s">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="2">
+        <v>13</v>
+      </c>
+      <c r="B16" s="2">
+        <v>2</v>
+      </c>
+      <c r="C16" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="D8" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>6</v>
-      </c>
-      <c r="B9">
-        <v>2</v>
-      </c>
-      <c r="C9" t="s">
+      <c r="D16" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="2">
+        <v>14</v>
+      </c>
+      <c r="B17" s="2">
+        <v>2</v>
+      </c>
+      <c r="C17" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="D9" t="s">
-        <v>72</v>
-      </c>
-      <c r="E9" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>7</v>
-      </c>
-      <c r="B10">
-        <v>2</v>
-      </c>
-      <c r="C10" t="s">
+      <c r="D17" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="2">
+        <v>15</v>
+      </c>
+      <c r="B18" s="2">
+        <v>2</v>
+      </c>
+      <c r="C18" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="D10" t="s">
-        <v>73</v>
-      </c>
-      <c r="E10" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>8</v>
-      </c>
-      <c r="B11">
-        <v>2</v>
-      </c>
-      <c r="C11" t="s">
+      <c r="D18" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="2">
+        <v>16</v>
+      </c>
+      <c r="B19" s="2">
+        <v>2</v>
+      </c>
+      <c r="C19" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="D11" t="s">
-        <v>74</v>
-      </c>
-      <c r="E11" t="s">
-        <v>88</v>
+      <c r="D19" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="2">
+        <v>17</v>
+      </c>
+      <c r="B20" s="2">
+        <v>2</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="2">
+        <v>18</v>
+      </c>
+      <c r="B21" s="2">
+        <v>2</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>102</v>
       </c>
     </row>
   </sheetData>
-  <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <mergeCells count="2">
     <mergeCell ref="A1:E1"/>
     <mergeCell ref="B2:C2"/>
   </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G25"/>
+  <dimension ref="A1:I50"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E54" sqref="E54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="3.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="3.42578125"/>
+    <col min="2" max="2" width="5.85546875"/>
+    <col min="3" max="3" width="9.5703125"/>
+    <col min="4" max="4" width="17"/>
+    <col min="5" max="5" width="20.7109375"/>
+    <col min="6" max="6" width="19.42578125"/>
+    <col min="7" max="7" width="30"/>
+    <col min="8" max="1025" width="9.42578125"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="C2" s="2"/>
+      <c r="B2" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="C2" s="3"/>
       <c r="D2" s="1" t="s">
-        <v>77</v>
+        <v>105</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>78</v>
+        <v>106</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>79</v>
+        <v>107</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
       <c r="B3" s="1" t="s">
         <v>1</v>
@@ -2150,452 +2388,1090 @@
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>1</v>
       </c>
-      <c r="B4">
-        <v>1</v>
-      </c>
-      <c r="C4" t="s">
+      <c r="B4" s="2">
+        <v>1</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="D4" t="s">
-        <v>81</v>
-      </c>
-      <c r="E4">
-        <v>1</v>
-      </c>
-      <c r="F4">
+      <c r="D4" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="E4" s="2">
+        <v>1</v>
+      </c>
+      <c r="F4" s="2">
         <v>20</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G4" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="H4" s="2"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>2</v>
       </c>
-      <c r="B5">
-        <v>1</v>
-      </c>
-      <c r="C5" t="s">
+      <c r="B5" s="2">
+        <v>1</v>
+      </c>
+      <c r="C5" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="D5" t="s">
-        <v>82</v>
-      </c>
-      <c r="E5">
-        <v>2</v>
-      </c>
-      <c r="F5">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D5" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="E5" s="2">
+        <v>6</v>
+      </c>
+      <c r="F5" s="2">
+        <v>20</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="H5" s="2"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>3</v>
       </c>
-      <c r="B6">
-        <v>1</v>
-      </c>
-      <c r="C6" t="s">
+      <c r="B6" s="2">
+        <v>1</v>
+      </c>
+      <c r="C6" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="D6" t="s">
-        <v>83</v>
-      </c>
-      <c r="E6">
-        <v>4</v>
-      </c>
-      <c r="F6">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D6" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="E6" s="2">
+        <v>12</v>
+      </c>
+      <c r="F6" s="2">
+        <v>14</v>
+      </c>
+      <c r="G6" s="2"/>
+      <c r="H6" s="2"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>4</v>
       </c>
-      <c r="B7">
-        <v>2</v>
-      </c>
-      <c r="C7" t="s">
-        <v>68</v>
-      </c>
-      <c r="D7" t="s">
-        <v>81</v>
-      </c>
-      <c r="E7">
-        <v>1</v>
-      </c>
-      <c r="F7">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B7" s="2">
+        <v>2</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="E7" s="2">
+        <v>1</v>
+      </c>
+      <c r="F7" s="2">
+        <v>16</v>
+      </c>
+      <c r="G7" s="2"/>
+      <c r="H7" s="2"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>5</v>
       </c>
-      <c r="B8">
-        <v>2</v>
-      </c>
-      <c r="C8" t="s">
-        <v>68</v>
-      </c>
-      <c r="D8" t="s">
-        <v>82</v>
-      </c>
-      <c r="E8">
-        <v>2</v>
-      </c>
-      <c r="F8">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B8" s="2">
+        <v>2</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="E8" s="2">
+        <v>3</v>
+      </c>
+      <c r="F8" s="2">
+        <v>16</v>
+      </c>
+      <c r="G8" s="2"/>
+      <c r="H8" s="2"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>6</v>
       </c>
-      <c r="B9">
-        <v>2</v>
-      </c>
-      <c r="C9" t="s">
-        <v>68</v>
-      </c>
-      <c r="D9" t="s">
-        <v>83</v>
-      </c>
-      <c r="E9">
-        <v>4</v>
-      </c>
-      <c r="F9">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B9" s="2">
+        <v>2</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="E9" s="2">
+        <v>6</v>
+      </c>
+      <c r="F9" s="2">
+        <v>16</v>
+      </c>
+      <c r="G9" s="2"/>
+      <c r="H9" s="2"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>7</v>
       </c>
-      <c r="B10">
-        <v>3</v>
-      </c>
-      <c r="C10" t="s">
-        <v>69</v>
-      </c>
-      <c r="D10" t="s">
-        <v>81</v>
-      </c>
-      <c r="E10">
-        <v>1</v>
-      </c>
-      <c r="F10">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B10" s="2">
+        <v>3</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="E10" s="2">
+        <v>1</v>
+      </c>
+      <c r="F10" s="2">
+        <v>22</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="H10" s="2"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>8</v>
       </c>
-      <c r="B11">
-        <v>3</v>
-      </c>
-      <c r="C11" t="s">
-        <v>69</v>
-      </c>
-      <c r="D11" t="s">
-        <v>82</v>
-      </c>
-      <c r="E11">
-        <v>2</v>
-      </c>
-      <c r="F11">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B11" s="2">
+        <v>3</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="E11" s="2">
+        <v>3</v>
+      </c>
+      <c r="F11" s="2">
+        <v>20</v>
+      </c>
+      <c r="G11" s="2"/>
+      <c r="H11" s="2"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>9</v>
       </c>
-      <c r="B12">
-        <v>3</v>
-      </c>
-      <c r="C12" t="s">
-        <v>69</v>
-      </c>
-      <c r="D12" t="s">
-        <v>83</v>
-      </c>
-      <c r="E12">
-        <v>4</v>
-      </c>
-      <c r="F12">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B12" s="2">
+        <v>3</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="E12" s="2">
+        <v>6</v>
+      </c>
+      <c r="F12" s="2">
+        <v>12</v>
+      </c>
+      <c r="G12" s="2"/>
+      <c r="H12" s="2"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>10</v>
       </c>
-      <c r="B13">
+      <c r="B13" s="2">
         <v>4</v>
       </c>
-      <c r="C13" t="s">
-        <v>70</v>
-      </c>
-      <c r="D13" t="s">
-        <v>81</v>
-      </c>
-      <c r="E13">
-        <v>1</v>
-      </c>
-      <c r="F13">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C13" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="E13" s="2">
+        <v>1</v>
+      </c>
+      <c r="F13" s="2">
+        <v>8</v>
+      </c>
+      <c r="G13" s="2"/>
+      <c r="H13" s="2"/>
+      <c r="I13" s="2"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>11</v>
       </c>
-      <c r="B14">
-        <v>4</v>
-      </c>
-      <c r="C14" t="s">
-        <v>70</v>
-      </c>
-      <c r="D14" t="s">
-        <v>82</v>
-      </c>
-      <c r="E14">
-        <v>2</v>
-      </c>
-      <c r="F14">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B14" s="2">
+        <v>5</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="E14" s="2">
+        <v>1</v>
+      </c>
+      <c r="F14" s="2">
+        <v>16</v>
+      </c>
+      <c r="G14" s="2"/>
+      <c r="H14" s="2"/>
+      <c r="I14" s="2"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>12</v>
       </c>
-      <c r="B15">
-        <v>4</v>
-      </c>
-      <c r="C15" t="s">
-        <v>70</v>
-      </c>
-      <c r="D15" t="s">
-        <v>83</v>
-      </c>
-      <c r="E15">
-        <v>4</v>
-      </c>
-      <c r="F15">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B15" s="2">
+        <v>5</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="E15" s="2">
+        <v>1</v>
+      </c>
+      <c r="F15" s="2">
+        <v>24</v>
+      </c>
+      <c r="G15" s="2"/>
+      <c r="H15" s="2"/>
+      <c r="I15" s="2"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>13</v>
       </c>
-      <c r="B16">
+      <c r="B16" s="2">
         <v>5</v>
       </c>
-      <c r="C16" t="s">
-        <v>71</v>
-      </c>
-      <c r="D16" t="s">
-        <v>81</v>
-      </c>
-      <c r="E16">
-        <v>1</v>
-      </c>
-      <c r="F16">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C16" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="E16" s="2">
+        <v>2</v>
+      </c>
+      <c r="F16" s="2">
+        <v>16</v>
+      </c>
+      <c r="G16" s="2"/>
+      <c r="H16" s="2"/>
+      <c r="I16" s="2"/>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>14</v>
       </c>
-      <c r="B17">
-        <v>5</v>
-      </c>
-      <c r="C17" t="s">
-        <v>71</v>
-      </c>
-      <c r="D17" t="s">
-        <v>82</v>
-      </c>
-      <c r="E17">
-        <v>2</v>
-      </c>
-      <c r="F17">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B17" s="2">
+        <v>6</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="E17" s="2">
+        <v>1</v>
+      </c>
+      <c r="F17" s="2">
+        <v>16</v>
+      </c>
+      <c r="G17" s="2"/>
+      <c r="H17" s="2"/>
+      <c r="I17" s="2"/>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>15</v>
       </c>
-      <c r="B18">
-        <v>5</v>
-      </c>
-      <c r="C18" t="s">
-        <v>71</v>
-      </c>
-      <c r="D18" t="s">
-        <v>83</v>
-      </c>
-      <c r="E18">
-        <v>4</v>
-      </c>
-      <c r="F18">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B18" s="2">
+        <v>6</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="E18" s="2">
+        <v>1</v>
+      </c>
+      <c r="F18" s="2">
+        <v>24</v>
+      </c>
+      <c r="G18" s="2"/>
+      <c r="H18" s="2"/>
+      <c r="I18" s="2"/>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>16</v>
       </c>
-      <c r="B19">
+      <c r="B19" s="2">
         <v>6</v>
       </c>
-      <c r="C19" t="s">
-        <v>72</v>
-      </c>
-      <c r="D19" t="s">
-        <v>81</v>
-      </c>
-      <c r="E19">
-        <v>1</v>
-      </c>
-      <c r="F19">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C19" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="E19" s="2">
+        <v>2</v>
+      </c>
+      <c r="F19" s="2">
+        <v>16</v>
+      </c>
+      <c r="G19" s="2"/>
+      <c r="H19" s="2"/>
+      <c r="I19" s="2"/>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>17</v>
       </c>
-      <c r="B20">
-        <v>6</v>
-      </c>
-      <c r="C20" t="s">
-        <v>72</v>
-      </c>
-      <c r="D20" t="s">
-        <v>82</v>
-      </c>
-      <c r="E20">
-        <v>2</v>
-      </c>
-      <c r="F20">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B20" s="2">
+        <v>7</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="E20" s="2">
+        <v>1</v>
+      </c>
+      <c r="F20" s="2">
+        <v>16</v>
+      </c>
+      <c r="G20" s="2"/>
+      <c r="H20" s="2"/>
+      <c r="I20" s="2"/>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>18</v>
       </c>
-      <c r="B21">
-        <v>6</v>
-      </c>
-      <c r="C21" t="s">
-        <v>72</v>
-      </c>
-      <c r="D21" t="s">
-        <v>83</v>
-      </c>
-      <c r="E21">
-        <v>4</v>
-      </c>
-      <c r="F21">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B21" s="2">
+        <v>7</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="E21" s="2">
+        <v>1</v>
+      </c>
+      <c r="F21" s="2">
+        <v>24</v>
+      </c>
+      <c r="G21" s="2"/>
+      <c r="H21" s="2"/>
+      <c r="I21" s="2"/>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>19</v>
       </c>
-      <c r="B22">
+      <c r="B22" s="2">
         <v>7</v>
       </c>
-      <c r="C22" t="s">
-        <v>73</v>
-      </c>
-      <c r="D22" t="s">
-        <v>82</v>
-      </c>
-      <c r="E22">
-        <v>4</v>
-      </c>
-      <c r="F22">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C22" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="E22" s="2">
+        <v>2</v>
+      </c>
+      <c r="F22" s="2">
+        <v>16</v>
+      </c>
+      <c r="G22" s="2"/>
+      <c r="H22" s="2"/>
+      <c r="I22" s="2"/>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>20</v>
       </c>
-      <c r="B23">
+      <c r="B23" s="2">
         <v>8</v>
       </c>
-      <c r="C23" t="s">
-        <v>74</v>
-      </c>
-      <c r="D23" t="s">
+      <c r="C23" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="E23">
-        <v>1</v>
-      </c>
-      <c r="F23">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D23" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="E23" s="2">
+        <v>1</v>
+      </c>
+      <c r="F23" s="2">
+        <v>16</v>
+      </c>
+      <c r="G23" s="2"/>
+      <c r="H23" s="2"/>
+      <c r="I23" s="2"/>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>21</v>
       </c>
-      <c r="B24">
+      <c r="B24" s="2">
         <v>8</v>
       </c>
-      <c r="C24" t="s">
-        <v>74</v>
-      </c>
-      <c r="D24" t="s">
-        <v>82</v>
-      </c>
-      <c r="E24">
-        <v>2</v>
-      </c>
-      <c r="F24">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C24" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="E24" s="2">
+        <v>1</v>
+      </c>
+      <c r="F24" s="2">
+        <v>24</v>
+      </c>
+      <c r="G24" s="2"/>
+      <c r="H24" s="2"/>
+      <c r="I24" s="2"/>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>22</v>
       </c>
-      <c r="B25">
+      <c r="B25" s="2">
         <v>8</v>
       </c>
-      <c r="C25" t="s">
-        <v>74</v>
-      </c>
-      <c r="D25" t="s">
+      <c r="C25" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="E25" s="2">
+        <v>2</v>
+      </c>
+      <c r="F25" s="2">
+        <v>16</v>
+      </c>
+      <c r="G25" s="2"/>
+      <c r="H25" s="2"/>
+      <c r="I25" s="2"/>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>23</v>
+      </c>
+      <c r="B26" s="2">
+        <v>9</v>
+      </c>
+      <c r="C26" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="E25">
+      <c r="D26" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="E26" s="2">
+        <v>1</v>
+      </c>
+      <c r="F26" s="2">
+        <v>20</v>
+      </c>
+      <c r="G26" s="2"/>
+      <c r="H26" s="2"/>
+      <c r="I26" s="2"/>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>24</v>
+      </c>
+      <c r="B27" s="2">
+        <v>9</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="E27" s="2">
         <v>4</v>
       </c>
-      <c r="F25">
+      <c r="F27" s="2">
+        <v>20</v>
+      </c>
+      <c r="G27" s="2"/>
+      <c r="H27" s="2"/>
+      <c r="I27" s="2"/>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>25</v>
+      </c>
+      <c r="B28" s="2">
+        <v>10</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="E28" s="2">
+        <v>1</v>
+      </c>
+      <c r="F28" s="2">
+        <v>20</v>
+      </c>
+      <c r="G28" s="2"/>
+      <c r="H28" s="2"/>
+      <c r="I28" s="2"/>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>26</v>
+      </c>
+      <c r="B29" s="2">
+        <v>10</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="E29" s="2">
+        <v>2</v>
+      </c>
+      <c r="F29" s="2">
+        <v>8</v>
+      </c>
+      <c r="G29" s="2"/>
+      <c r="H29" s="2"/>
+      <c r="I29" s="2"/>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>27</v>
+      </c>
+      <c r="B30" s="2">
+        <v>10</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="E30" s="2">
+        <v>4</v>
+      </c>
+      <c r="F30" s="2">
+        <v>20</v>
+      </c>
+      <c r="G30" s="2"/>
+      <c r="H30" s="2"/>
+      <c r="I30" s="2"/>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>28</v>
+      </c>
+      <c r="B31" s="2">
+        <v>11</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="D31" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="E31" s="2">
+        <v>1</v>
+      </c>
+      <c r="F31" s="2">
+        <v>18</v>
+      </c>
+      <c r="G31" s="2"/>
+      <c r="H31" s="2"/>
+      <c r="I31" s="2"/>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>29</v>
+      </c>
+      <c r="B32" s="2">
+        <v>11</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="D32" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="E32" s="2">
+        <v>2</v>
+      </c>
+      <c r="F32" s="2">
+        <v>18</v>
+      </c>
+      <c r="G32" s="2"/>
+      <c r="H32" s="2"/>
+      <c r="I32" s="2"/>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>30</v>
+      </c>
+      <c r="B33" s="2">
+        <v>11</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="D33" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="E33" s="2">
+        <v>4</v>
+      </c>
+      <c r="F33" s="2">
+        <v>12</v>
+      </c>
+      <c r="G33" s="2"/>
+      <c r="H33" s="2"/>
+      <c r="I33" s="2"/>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>31</v>
+      </c>
+      <c r="B34" s="2">
+        <v>12</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="D34" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="E34" s="2">
+        <v>1</v>
+      </c>
+      <c r="F34" s="2">
+        <v>18</v>
+      </c>
+      <c r="G34" s="2"/>
+      <c r="H34" s="2"/>
+      <c r="I34" s="2"/>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>32</v>
+      </c>
+      <c r="B35" s="2">
+        <v>12</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="D35" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="E35" s="2">
+        <v>1</v>
+      </c>
+      <c r="F35" s="2">
+        <v>18</v>
+      </c>
+      <c r="G35" s="2"/>
+      <c r="H35" s="2"/>
+      <c r="I35" s="2"/>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>33</v>
+      </c>
+      <c r="B36" s="2">
+        <v>12</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="D36" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="E36" s="2">
+        <v>2</v>
+      </c>
+      <c r="F36" s="2">
+        <v>12</v>
+      </c>
+      <c r="G36" s="2"/>
+      <c r="H36" s="2"/>
+      <c r="I36" s="2"/>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>34</v>
+      </c>
+      <c r="B37" s="2">
+        <v>13</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="D37" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="E37" s="2">
+        <v>1</v>
+      </c>
+      <c r="F37" s="2">
+        <v>16</v>
+      </c>
+      <c r="G37" s="2"/>
+      <c r="H37" s="2"/>
+      <c r="I37" s="2"/>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>35</v>
+      </c>
+      <c r="B38" s="2">
+        <v>13</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="D38" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="E38" s="2">
+        <v>2</v>
+      </c>
+      <c r="F38" s="2">
+        <v>4</v>
+      </c>
+      <c r="G38" s="2"/>
+      <c r="H38" s="2"/>
+      <c r="I38" s="2"/>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>36</v>
+      </c>
+      <c r="B39" s="2">
+        <v>13</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="D39" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="E39" s="2">
+        <v>2</v>
+      </c>
+      <c r="F39" s="2">
+        <v>12</v>
+      </c>
+      <c r="G39" s="2"/>
+      <c r="H39" s="2"/>
+      <c r="I39" s="2"/>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>37</v>
+      </c>
+      <c r="B40" s="2">
+        <v>14</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="D40" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="E40" s="2">
+        <v>1</v>
+      </c>
+      <c r="F40" s="2">
+        <v>16</v>
+      </c>
+      <c r="G40" s="2"/>
+      <c r="H40" s="2"/>
+      <c r="I40" s="2"/>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>38</v>
+      </c>
+      <c r="B41" s="2">
+        <v>14</v>
+      </c>
+      <c r="C41" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="D41" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="E41" s="2">
+        <v>2</v>
+      </c>
+      <c r="F41" s="2">
+        <v>16</v>
+      </c>
+      <c r="G41" s="2"/>
+      <c r="H41" s="2"/>
+      <c r="I41" s="2"/>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>39</v>
+      </c>
+      <c r="B42" s="2">
+        <v>15</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="D42" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="E42" s="2">
+        <v>1</v>
+      </c>
+      <c r="F42" s="2">
+        <v>12</v>
+      </c>
+      <c r="G42" s="2"/>
+      <c r="H42" s="2"/>
+      <c r="I42" s="2"/>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <v>40</v>
+      </c>
+      <c r="B43" s="2">
+        <v>15</v>
+      </c>
+      <c r="C43" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="D43" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="E43" s="2">
+        <v>2</v>
+      </c>
+      <c r="F43" s="2">
+        <v>20</v>
+      </c>
+      <c r="G43" s="2"/>
+      <c r="H43" s="2"/>
+      <c r="I43" s="2"/>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <v>41</v>
+      </c>
+      <c r="B44" s="2">
+        <v>16</v>
+      </c>
+      <c r="C44" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="D44" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="E44" s="2">
+        <v>1</v>
+      </c>
+      <c r="F44" s="2">
+        <v>14</v>
+      </c>
+      <c r="G44" s="2"/>
+      <c r="H44" s="2"/>
+      <c r="I44" s="2"/>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <v>42</v>
+      </c>
+      <c r="B45" s="2">
+        <v>16</v>
+      </c>
+      <c r="C45" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="D45" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="E45" s="2">
+        <v>2</v>
+      </c>
+      <c r="F45" s="2">
+        <v>18</v>
+      </c>
+      <c r="G45" s="2"/>
+      <c r="H45" s="2"/>
+      <c r="I45" s="2"/>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A46">
+        <v>43</v>
+      </c>
+      <c r="B46" s="2">
+        <v>17</v>
+      </c>
+      <c r="C46" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="D46" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="E46" s="2">
+        <v>1</v>
+      </c>
+      <c r="F46" s="2">
+        <v>10</v>
+      </c>
+      <c r="G46" s="2"/>
+      <c r="H46" s="2"/>
+      <c r="I46" s="2"/>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A47">
+        <v>44</v>
+      </c>
+      <c r="B47" s="2">
+        <v>17</v>
+      </c>
+      <c r="C47" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="D47" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="E47" s="2">
+        <v>2</v>
+      </c>
+      <c r="F47" s="2">
         <v>22</v>
       </c>
+      <c r="G47" s="2"/>
+      <c r="H47" s="2"/>
+      <c r="I47" s="2"/>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A48">
+        <v>45</v>
+      </c>
+      <c r="B48" s="2">
+        <v>18</v>
+      </c>
+      <c r="C48" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="D48" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="E48" s="2">
+        <v>1</v>
+      </c>
+      <c r="F48" s="2">
+        <v>6</v>
+      </c>
+      <c r="G48" s="2"/>
+      <c r="H48" s="2"/>
+      <c r="I48" s="2"/>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A49">
+        <v>46</v>
+      </c>
+      <c r="B49" s="2">
+        <v>18</v>
+      </c>
+      <c r="C49" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="D49" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="E49" s="2">
+        <v>2</v>
+      </c>
+      <c r="F49" s="2">
+        <v>10</v>
+      </c>
+      <c r="G49" s="2"/>
+      <c r="H49" s="2"/>
+      <c r="I49" s="2"/>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A50">
+        <v>47</v>
+      </c>
+      <c r="B50" s="2">
+        <v>18</v>
+      </c>
+      <c r="C50" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="D50" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="E50" s="2">
+        <v>2</v>
+      </c>
+      <c r="F50" s="2">
+        <v>16</v>
+      </c>
+      <c r="G50" s="2"/>
+      <c r="H50" s="2"/>
+      <c r="I50" s="2"/>
     </row>
   </sheetData>
-  <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <mergeCells count="2">
     <mergeCell ref="A1:G1"/>
     <mergeCell ref="B2:C2"/>
   </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Fix import sur les utilisateurs
</commit_message>
<xml_diff>
--- a/Fixtures.xlsx
+++ b/Fixtures.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="5"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Liste des Composantes" sheetId="1" state="visible" r:id="rId2"/>
@@ -147,7 +147,7 @@
     <t xml:space="preserve">$2y$15$.T2Hlu8.6AdOKCvqsUCRkenMxGtaM8zeoVsCKzzZ1ocBSvW27dHV.</t>
   </si>
   <si>
-    <t xml:space="preserve">www.google.fr</t>
+    <t xml:space="preserve">http://www.google.fr</t>
   </si>
   <si>
     <t xml:space="preserve">charp.antoine@gmail.com</t>
@@ -482,14 +482,13 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="A1:G50"/>
+      <selection pane="topLeft" activeCell="B2" activeCellId="1" sqref="I9:I19 B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="3.55465587044534"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="7.44939271255061"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="9.69230769230769"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="3.62753036437247"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="7.71255060728745"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -544,15 +543,14 @@
   <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="A1:G50"/>
+      <selection pane="topLeft" activeCell="C2" activeCellId="1" sqref="I9:I19 C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="3.55465587044534"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="41.5991902834008"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="35.336032388664"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="9.69230769230769"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="3.62753036437247"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="43.0485829959514"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="36.5222672064777"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -671,29 +669,28 @@
   </sheetPr>
   <dimension ref="A1:Q19"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="Q3" activeCellId="1" sqref="A1:G50 Q3"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="H1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I9" activeCellId="0" sqref="I9:I19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="3.55465587044534"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="7.44939271255061"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="22.5465587044534"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="12.5263157894737"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="22.5465587044534"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="90.8380566801619"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="8.57085020242915"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="17.4655870445344"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="3.55465587044534"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="28.8704453441295"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="3.55465587044534"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="28.8704453441295"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="3.55465587044534"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="31.4412955465587"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="3.55465587044534"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="18.7894736842105"/>
-    <col collapsed="false" hidden="false" max="1025" min="18" style="0" width="9.69230769230769"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="3.62753036437247"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="7.71255060728745"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="23.2753036437247"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="12.919028340081"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="23.2753036437247"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="94.0647773279352"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="8.89878542510122"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="18.0607287449393"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="3.62753036437247"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="29.8663967611336"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="3.62753036437247"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="29.8663967611336"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="3.62753036437247"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="32.5627530364372"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="3.62753036437247"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="19.4453441295547"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1052,7 +1049,7 @@
         <v>33222113344</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="n">
         <v>2</v>
       </c>
@@ -1105,7 +1102,7 @@
         <v>33222113344</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="n">
         <v>2</v>
       </c>
@@ -1158,7 +1155,7 @@
         <v>33222113344</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="n">
         <v>2</v>
       </c>
@@ -1211,7 +1208,7 @@
         <v>33222113344</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="n">
         <v>3</v>
       </c>
@@ -1264,7 +1261,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="n">
         <v>3</v>
       </c>
@@ -1317,7 +1314,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="n">
         <v>3</v>
       </c>
@@ -1370,7 +1367,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="n">
         <v>3</v>
       </c>
@@ -1423,7 +1420,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="n">
         <v>4</v>
       </c>
@@ -1476,7 +1473,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="n">
         <v>4</v>
       </c>
@@ -1529,7 +1526,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="n">
         <v>4</v>
       </c>
@@ -1582,7 +1579,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="n">
         <v>4</v>
       </c>
@@ -1662,17 +1659,16 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F6" activeCellId="0" sqref="A1:G50"/>
+      <selection pane="topLeft" activeCell="F6" activeCellId="1" sqref="I9:I19 F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="3.55465587044534"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="7.44939271255061"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="3.55465587044534"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="9.81781376518219"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="14.9595141700405"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="9.69230769230769"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="3.62753036437247"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="7.71255060728745"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="3.62753036437247"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="10.085020242915"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="15.4251012145749"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1761,16 +1757,15 @@
   <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E26" activeCellId="0" sqref="A1:G50"/>
+      <selection pane="topLeft" activeCell="E26" activeCellId="1" sqref="I9:I19 E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="3.55465587044534"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="10.6032388663968"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="9.81781376518219"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="56.8866396761134"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="9.69230769230769"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="3.62753036437247"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="10.9392712550607"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="10.085020242915"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="58.8663967611336"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2136,20 +2131,19 @@
   </sheetPr>
   <dimension ref="A1:G50"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1:G50"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="I9:I19 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="3.55465587044534"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="6"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="9.81781376518219"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="17.4655870445344"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="21.4251012145749"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="20.0364372469636"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="31.0485829959514"/>
-    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="9.69230769230769"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="3.62753036437247"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="6.19838056680162"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="10.085020242915"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="18.0607287449393"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="22.1538461538462"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="20.7651821862348"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="32.1012145748988"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>